<commit_message>
Versão SNCT OFC - Incompleta
</commit_message>
<xml_diff>
--- a/catalogacaoDados.xlsx
+++ b/catalogacaoDados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jovan\Downloads\Catalogação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6b5bbdbba8571144/Documentos/Catalogação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21429E2-6FC2-4411-A791-4E73B5425901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="203" documentId="13_ncr:1_{B5095B00-5C27-4C5C-A4AC-E86D5CF29E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E39E0E7-7ADD-4200-8E7E-26715AEC1DCF}"/>
   <bookViews>
-    <workbookView xWindow="3336" yWindow="1944" windowWidth="17280" windowHeight="8880" xr2:uid="{647034AA-FDB6-4D4C-869C-9BA5C3A85442}"/>
+    <workbookView xWindow="2640" yWindow="1248" windowWidth="17280" windowHeight="8880" xr2:uid="{647034AA-FDB6-4D4C-869C-9BA5C3A85442}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="240">
   <si>
     <t>Cajueiro</t>
   </si>
@@ -762,6 +762,33 @@
     <t>https://maps.app.goo.gl/hdG9mRSMpfzGEGs121</t>
   </si>
   <si>
+    <t>Guará</t>
+  </si>
+  <si>
+    <t>Eudocimus ruber</t>
+  </si>
+  <si>
+    <t>Guara</t>
+  </si>
+  <si>
+    <t>imgs\especies\Guará\1.jpg</t>
+  </si>
+  <si>
+    <t>imgs\especies\Guará\1.mp4</t>
+  </si>
+  <si>
+    <t>O Eudocimus ruber, conhecido como guará-vermelho, é uma ave nativa de regiões costeiras e zonas úmidas, como manguezais e áreas de restinga. Ele é facilmente reconhecido por sua plumagem vibrante de cor vermelha, que é obtida através de sua dieta rica em crustáceos, como os caranguejos. O guará-vermelho desempenha um papel ecológico importante, ajudando a controlar as populações de crustáceos em manguezais. Além disso, sua presença nesses ecossistemas é um indicativo de boa saúde ambiental, já que essas aves dependem de áreas úmidas bem preservadas para se alimentar e se reproduzir.</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/hdG9mRSMpfzGEGs122</t>
+  </si>
+  <si>
+    <t>Threskiornithidae</t>
+  </si>
+  <si>
+    <t>Eudocimus</t>
+  </si>
+  <si>
     <t>Tralhoto</t>
   </si>
   <si>
@@ -777,20 +804,20 @@
     <t>O Anableps anableps, conhecido popularmente como tralhoto ou peixe-de-quatro-olhos, é um peixe de água doce encontrado em ambientes costeiros, como estuários e manguezais da América do Sul. Este peixe é notável por suas adaptações únicas, incluindo olhos que se dividem em duas partes, permitindo que ele veja tanto acima quanto abaixo da superfície da água ao mesmo tempo. O tralhoto se alimenta de insetos, pequenos crustáceos e matéria orgânica, desempenhando um papel importante na cadeia alimentar desses ecossistemas. Sua presença em áreas de manguezais contribui para a biodiversidade local e é um indicativo da saúde dos ambientes aquáticos em que habita.</t>
   </si>
   <si>
+    <t>https://maps.app.goo.gl/hdG9mRSMpfzGEGs123</t>
+  </si>
+  <si>
     <t>Anablepidae</t>
   </si>
   <si>
     <t>Four-eyed fish</t>
-  </si>
-  <si>
-    <t>https://maps.app.goo.gl/hdG9mRSMpfzGEGs123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -862,13 +889,6 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -897,7 +917,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -921,9 +941,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1261,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65009DD9-AB6C-4675-B464-E2784F87AEDE}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8"/>
@@ -2241,36 +2258,68 @@
         <v>222</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="28.2" customHeight="1">
+    <row r="31" spans="1:10" ht="42.6" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>223</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>224</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="H31" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="I31" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>230</v>
+    </row>
+    <row r="32" spans="1:10" ht="28.2" customHeight="1">
+      <c r="A32" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2304,9 +2353,10 @@
     <hyperlink ref="J28" r:id="rId26" display="https://maps.app.goo.gl/hdG9mRSMpfzGEGs96" xr:uid="{2C7221DF-102A-479A-A447-4806655E5DF9}"/>
     <hyperlink ref="J29" r:id="rId27" display="https://maps.app.goo.gl/hdG9mRSMpfzGEGs96" xr:uid="{C88C4B0F-589C-441B-9F3C-B61DEBC17FE2}"/>
     <hyperlink ref="J30" r:id="rId28" display="https://maps.app.goo.gl/hdG9mRSMpfzGEGs96" xr:uid="{373ED401-B2F9-4B85-86C0-5E587F8DB454}"/>
-    <hyperlink ref="J31" r:id="rId29" display="https://maps.app.goo.gl/hdG9mRSMpfzGEGs96" xr:uid="{B6BB9840-E90B-46C3-B4EB-6D22709BD96C}"/>
+    <hyperlink ref="J31" r:id="rId29" display="https://maps.app.goo.gl/hdG9mRSMpfzGEGs96" xr:uid="{8E15DE48-F702-4E11-86B6-1741DF1C1A23}"/>
+    <hyperlink ref="J32" r:id="rId30" display="https://maps.app.goo.gl/hdG9mRSMpfzGEGs96" xr:uid="{E46EBD89-187C-4047-B5B1-7BE926CD33FD}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>